<commit_message>
add male for fleeting
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -122,7 +122,12 @@
     <t>Player</t>
   </si>
   <si>
-    <t>Prefabs/Object/Alch_plate</t>
+    <t>Prefabs/Object/Player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Male100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -520,7 +525,7 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L5"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -813,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="V4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.15">
@@ -881,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="V5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add drop item list record
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="19560" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,14 +20,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Item" type="4" background="1" refreshedVersion="2" saveData="1">
-    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Item.xml" htmlFormat="all" htmlTables="1"/>
+  <connection id="1" name="Item" type="4" refreshedVersion="2" background="1" saveData="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Item.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -124,19 +129,17 @@
   </si>
   <si>
     <t>Enemy</t>
+  </si>
+  <si>
+    <t>DropPack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -144,7 +147,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -166,23 +169,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -194,14 +182,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -500,6 +493,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -532,15 +526,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:V8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -561,7 +554,7 @@
     <col min="22" max="22" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -628,8 +621,11 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -697,7 +693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -765,7 +761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -833,7 +829,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -901,7 +897,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -969,20 +965,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
add NPC move type
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -125,7 +125,27 @@
     <t>Enemy</t>
   </si>
   <si>
-    <t>DropPack</t>
+    <t>DropPackList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>tkDis</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -133,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -143,6 +163,13 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -168,11 +195,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -521,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -546,10 +576,12 @@
     <col min="16" max="16" width="12" customWidth="1"/>
     <col min="17" max="17" width="14.25" customWidth="1"/>
     <col min="21" max="21" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.125" customWidth="1"/>
+    <col min="22" max="22" width="25" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="25" customWidth="1"/>
+    <col min="25" max="25" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -617,10 +649,16 @@
         <v>21</v>
       </c>
       <c r="W1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -687,8 +725,14 @@
       <c r="V2" t="s">
         <v>30</v>
       </c>
+      <c r="W2">
+        <v>2</v>
+      </c>
+      <c r="X2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -755,8 +799,14 @@
       <c r="V3" t="s">
         <v>30</v>
       </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -823,8 +873,14 @@
       <c r="V4" t="s">
         <v>30</v>
       </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -891,8 +947,14 @@
       <c r="V5" t="s">
         <v>30</v>
       </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -959,14 +1021,20 @@
       <c r="V6" t="s">
         <v>30</v>
       </c>
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>

</xml_diff>

<commit_message>
fix NPC HP error
Former-commit-id: b33ca7762dfbbb1354a357654fd255991fa48307 [formerly 9f62ea864a144eeb6c017bfb890177b54fae3dfe]
Former-commit-id: af75c8c4359c7f5c0e7d5fb737111e7cef184122
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -146,6 +146,10 @@
       </rPr>
       <t>tkDis</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAXHP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -564,24 +568,24 @@
     <col min="3" max="3" width="9.375" customWidth="1"/>
     <col min="4" max="4" width="12.75" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="8" max="8" width="25.25" customWidth="1"/>
-    <col min="9" max="9" width="15.125" customWidth="1"/>
-    <col min="10" max="10" width="16.875" customWidth="1"/>
-    <col min="11" max="11" width="14.625" customWidth="1"/>
-    <col min="12" max="12" width="16.75" customWidth="1"/>
-    <col min="13" max="13" width="22" customWidth="1"/>
-    <col min="14" max="14" width="16.75" customWidth="1"/>
-    <col min="15" max="15" width="13.25" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="17" width="14.25" customWidth="1"/>
-    <col min="21" max="21" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="25" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="25" customWidth="1"/>
-    <col min="25" max="25" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="25.25" customWidth="1"/>
+    <col min="10" max="10" width="15.125" customWidth="1"/>
+    <col min="11" max="11" width="16.875" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="13" max="13" width="16.75" customWidth="1"/>
+    <col min="14" max="14" width="22" customWidth="1"/>
+    <col min="15" max="15" width="16.75" customWidth="1"/>
+    <col min="16" max="16" width="13.25" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="14.25" customWidth="1"/>
+    <col min="22" max="22" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="25" customWidth="1"/>
+    <col min="26" max="26" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,64 +605,67 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -681,26 +688,26 @@
         <v>200</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>50</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>40</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>55000</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>10000</v>
       </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
       <c r="O2">
         <v>10</v>
       </c>
@@ -711,7 +718,7 @@
         <v>10</v>
       </c>
       <c r="R2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S2">
         <v>5</v>
@@ -722,17 +729,20 @@
       <c r="U2">
         <v>5</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2">
+        <v>5</v>
+      </c>
+      <c r="W2" t="s">
         <v>30</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>2</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -755,26 +765,26 @@
         <v>400</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>100</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>60</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>55000</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>10000</v>
       </c>
-      <c r="N3">
-        <v>10</v>
-      </c>
       <c r="O3">
         <v>10</v>
       </c>
@@ -785,7 +795,7 @@
         <v>10</v>
       </c>
       <c r="R3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S3">
         <v>5</v>
@@ -796,17 +806,20 @@
       <c r="U3">
         <v>5</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3">
+        <v>5</v>
+      </c>
+      <c r="W3" t="s">
         <v>30</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>2</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -829,26 +842,26 @@
         <v>600</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>150</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>80</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>55000</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>10000</v>
       </c>
-      <c r="N4">
-        <v>10</v>
-      </c>
       <c r="O4">
         <v>10</v>
       </c>
@@ -859,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="R4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S4">
         <v>5</v>
@@ -870,17 +883,20 @@
       <c r="U4">
         <v>5</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4">
+        <v>5</v>
+      </c>
+      <c r="W4" t="s">
         <v>30</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>2</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -903,26 +919,26 @@
         <v>600</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>150</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>80</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>55000</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>10000</v>
       </c>
-      <c r="N5">
-        <v>10</v>
-      </c>
       <c r="O5">
         <v>10</v>
       </c>
@@ -933,7 +949,7 @@
         <v>10</v>
       </c>
       <c r="R5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S5">
         <v>5</v>
@@ -944,17 +960,20 @@
       <c r="U5">
         <v>5</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5" t="s">
         <v>30</v>
       </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
       <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -977,26 +996,26 @@
         <v>600</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>150</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>80</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>55000</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>10000</v>
       </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
       <c r="O6">
         <v>10</v>
       </c>
@@ -1007,7 +1026,7 @@
         <v>10</v>
       </c>
       <c r="R6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S6">
         <v>5</v>
@@ -1018,23 +1037,26 @@
       <c r="U6">
         <v>5</v>
       </c>
-      <c r="V6" t="s">
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6" t="s">
         <v>30</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>2</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>

</xml_diff>

<commit_message>
add default config for npc
Former-commit-id: 7a8c41d51dc09d8a14c0d0198b56552fbf5d360a [formerly 7f96058584dc2b1dc96c50eb0f1dcb246164130b]
Former-commit-id: 4f5c7291a56b8138b2536de27d477dec025dd617
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="19560" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <author>杨鹏博</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -39,14 +44,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Item" type="4" background="1" refreshedVersion="2" saveData="1">
-    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Item.xml" htmlFormat="all" htmlTables="1"/>
+  <connection id="1" name="Item" type="4" refreshedVersion="2" background="1" saveData="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Item.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -173,23 +178,22 @@
     <t>60</t>
   </si>
   <si>
-    <t>Player</t>
-  </si>
-  <si>
     <t>Enemy</t>
+  </si>
+  <si>
+    <t>Default</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player_0_0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -203,7 +207,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -225,23 +235,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -256,14 +251,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -562,6 +562,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -594,15 +595,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -621,12 +621,13 @@
     <col min="17" max="17" width="12" customWidth="1"/>
     <col min="18" max="18" width="14.25" customWidth="1"/>
     <col min="22" max="22" width="11.625" customWidth="1"/>
-    <col min="23" max="25" width="25" customWidth="1"/>
+    <col min="23" max="23" width="63.375" customWidth="1"/>
+    <col min="24" max="25" width="25" customWidth="1"/>
     <col min="26" max="26" width="13.875" customWidth="1"/>
     <col min="27" max="27" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -709,7 +710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -789,7 +790,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -869,7 +870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -949,9 +950,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>35</v>
@@ -1029,9 +1030,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -1109,21 +1110,96 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>600</v>
+      </c>
+      <c r="G7">
+        <v>600</v>
+      </c>
+      <c r="H7">
+        <v>600</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>150</v>
+      </c>
+      <c r="L7">
+        <v>80</v>
+      </c>
+      <c r="M7">
+        <v>55000</v>
+      </c>
+      <c r="N7">
+        <v>10000</v>
+      </c>
+      <c r="O7">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+      <c r="Q7">
+        <v>10</v>
+      </c>
+      <c r="R7">
+        <v>10</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>5</v>
+      </c>
+      <c r="V7">
+        <v>5</v>
+      </c>
+      <c r="W7" t="s">
+        <v>30</v>
+      </c>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>20</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
add hero configure file
Former-commit-id: 3c9e4df951a5eac422e207e0809a5612d750bdea [formerly aaf20e8ef3c40467e5d084a82097abdbfe3eaf51]
Former-commit-id: 84dc27d638fdbc178c87e7507695a46b74f50848
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
     <author>杨鹏博</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,14 +39,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Item" type="4" refreshedVersion="2" background="1" saveData="1">
-    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Item.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Item" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Item.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58">
   <si>
     <t>ID</t>
   </si>
@@ -151,21 +146,87 @@
     <t>SkillIDRef</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/Alch_plate</t>
+  </si>
+  <si>
+    <t>DropBag_1</t>
+  </si>
+  <si>
+    <t>Player_0_0</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/ActionHero</t>
+  </si>
+  <si>
+    <t>Player_0_1</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/ChopperPilot</t>
+  </si>
+  <si>
+    <t>Player_0_2</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/Hero</t>
+  </si>
+  <si>
+    <t>Player_0_3</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/Knight</t>
+  </si>
+  <si>
+    <t>Player_0_4</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/VietcongSoldier</t>
+  </si>
+  <si>
+    <t>Player_1_0</t>
+  </si>
+  <si>
+    <t>Player_1_1</t>
+  </si>
+  <si>
+    <t>Player_1_2</t>
+  </si>
+  <si>
+    <t>Player_1_3</t>
+  </si>
+  <si>
+    <t>Player_1_4</t>
+  </si>
+  <si>
+    <t>Player_2_0</t>
+  </si>
+  <si>
+    <t>Player_2_1</t>
+  </si>
+  <si>
+    <t>Player_2_2</t>
+  </si>
+  <si>
+    <t>Player_2_3</t>
+  </si>
+  <si>
+    <t>Player_2_4</t>
+  </si>
+  <si>
     <t>AttackNpc1</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Prefabs/Object/Alch_plate</t>
-  </si>
-  <si>
-    <t>DropBag_1</t>
-  </si>
-  <si>
     <t>AttackNpc2</t>
   </si>
   <si>
@@ -175,25 +236,20 @@
     <t>AttackNpc3</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
     <t>Enemy</t>
-  </si>
-  <si>
-    <t>Default</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Player_0_0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -201,19 +257,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -235,8 +279,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -247,23 +306,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -562,7 +616,6 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -595,14 +648,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -627,7 +681,7 @@
     <col min="27" max="27" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,7 +764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -727,13 +781,13 @@
         <v>28</v>
       </c>
       <c r="F2">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="G2">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="H2">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -742,10 +796,10 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="L2">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="M2">
         <v>55000</v>
@@ -790,12 +844,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="1" spans="1:26">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -804,16 +858,16 @@
         <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="H3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -822,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="L3">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M3">
         <v>55000</v>
@@ -858,10 +912,10 @@
         <v>5</v>
       </c>
       <c r="W3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="X3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <v>20</v>
@@ -870,12 +924,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="1" spans="1:26">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -884,7 +938,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F4">
         <v>600</v>
@@ -938,10 +992,10 @@
         <v>5</v>
       </c>
       <c r="W4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y4">
         <v>20</v>
@@ -950,12 +1004,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="1" spans="1:26">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -964,7 +1018,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F5">
         <v>600</v>
@@ -1018,7 +1072,7 @@
         <v>5</v>
       </c>
       <c r="W5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="X5">
         <v>0</v>
@@ -1030,12 +1084,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="1" spans="1:26">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1044,7 +1098,7 @@
         <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F6">
         <v>600</v>
@@ -1098,10 +1152,10 @@
         <v>5</v>
       </c>
       <c r="W6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="X6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <v>20</v>
@@ -1110,12 +1164,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="1" spans="1:26">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1124,7 +1178,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F7">
         <v>600</v>
@@ -1178,10 +1232,10 @@
         <v>5</v>
       </c>
       <c r="W7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="X7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <v>20</v>
@@ -1190,16 +1244,1129 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+    <row r="8" customFormat="1" spans="1:26">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>600</v>
+      </c>
+      <c r="G8">
+        <v>600</v>
+      </c>
+      <c r="H8">
+        <v>600</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>150</v>
+      </c>
+      <c r="L8">
+        <v>80</v>
+      </c>
+      <c r="M8">
+        <v>55000</v>
+      </c>
+      <c r="N8">
+        <v>10000</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>10</v>
+      </c>
+      <c r="Q8">
+        <v>10</v>
+      </c>
+      <c r="R8">
+        <v>10</v>
+      </c>
+      <c r="S8">
+        <v>5</v>
+      </c>
+      <c r="T8">
+        <v>5</v>
+      </c>
+      <c r="U8">
+        <v>5</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8" t="s">
+        <v>33</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>20</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" spans="1:26">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>600</v>
+      </c>
+      <c r="G9">
+        <v>600</v>
+      </c>
+      <c r="H9">
+        <v>600</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>150</v>
+      </c>
+      <c r="L9">
+        <v>80</v>
+      </c>
+      <c r="M9">
+        <v>55000</v>
+      </c>
+      <c r="N9">
+        <v>10000</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>10</v>
+      </c>
+      <c r="R9">
+        <v>10</v>
+      </c>
+      <c r="S9">
+        <v>5</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
+      </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9" t="s">
+        <v>35</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>20</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" spans="1:26">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>600</v>
+      </c>
+      <c r="G10">
+        <v>600</v>
+      </c>
+      <c r="H10">
+        <v>600</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>150</v>
+      </c>
+      <c r="L10">
+        <v>80</v>
+      </c>
+      <c r="M10">
+        <v>55000</v>
+      </c>
+      <c r="N10">
+        <v>10000</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>10</v>
+      </c>
+      <c r="Q10">
+        <v>10</v>
+      </c>
+      <c r="R10">
+        <v>10</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>5</v>
+      </c>
+      <c r="W10" t="s">
+        <v>37</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>20</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" spans="1:26">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>600</v>
+      </c>
+      <c r="G11">
+        <v>600</v>
+      </c>
+      <c r="H11">
+        <v>600</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>150</v>
+      </c>
+      <c r="L11">
+        <v>80</v>
+      </c>
+      <c r="M11">
+        <v>55000</v>
+      </c>
+      <c r="N11">
+        <v>10000</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
+      </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
+      <c r="T11">
+        <v>5</v>
+      </c>
+      <c r="U11">
+        <v>5</v>
+      </c>
+      <c r="V11">
+        <v>5</v>
+      </c>
+      <c r="W11" t="s">
+        <v>39</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>20</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" spans="1:26">
+      <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12">
+        <v>600</v>
+      </c>
+      <c r="G12">
+        <v>600</v>
+      </c>
+      <c r="H12">
+        <v>600</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>150</v>
+      </c>
+      <c r="L12">
+        <v>80</v>
+      </c>
+      <c r="M12">
+        <v>55000</v>
+      </c>
+      <c r="N12">
+        <v>10000</v>
+      </c>
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <v>10</v>
+      </c>
+      <c r="Q12">
+        <v>10</v>
+      </c>
+      <c r="R12">
+        <v>10</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <v>5</v>
+      </c>
+      <c r="U12">
+        <v>5</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+      <c r="W12" t="s">
+        <v>41</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>20</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" spans="1:26">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13">
+        <v>600</v>
+      </c>
+      <c r="G13">
+        <v>600</v>
+      </c>
+      <c r="H13">
+        <v>600</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>150</v>
+      </c>
+      <c r="L13">
+        <v>80</v>
+      </c>
+      <c r="M13">
+        <v>55000</v>
+      </c>
+      <c r="N13">
+        <v>10000</v>
+      </c>
+      <c r="O13">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <v>10</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13">
+        <v>10</v>
+      </c>
+      <c r="S13">
+        <v>5</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+      <c r="U13">
+        <v>5</v>
+      </c>
+      <c r="V13">
+        <v>5</v>
+      </c>
+      <c r="W13" t="s">
+        <v>33</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>20</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" spans="1:26">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>600</v>
+      </c>
+      <c r="G14">
+        <v>600</v>
+      </c>
+      <c r="H14">
+        <v>600</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>150</v>
+      </c>
+      <c r="L14">
+        <v>80</v>
+      </c>
+      <c r="M14">
+        <v>55000</v>
+      </c>
+      <c r="N14">
+        <v>10000</v>
+      </c>
+      <c r="O14">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <v>10</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
+      <c r="T14">
+        <v>5</v>
+      </c>
+      <c r="U14">
+        <v>5</v>
+      </c>
+      <c r="V14">
+        <v>5</v>
+      </c>
+      <c r="W14" t="s">
+        <v>35</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>20</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" spans="1:26">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15">
+        <v>600</v>
+      </c>
+      <c r="G15">
+        <v>600</v>
+      </c>
+      <c r="H15">
+        <v>600</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>150</v>
+      </c>
+      <c r="L15">
+        <v>80</v>
+      </c>
+      <c r="M15">
+        <v>55000</v>
+      </c>
+      <c r="N15">
+        <v>10000</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="T15">
+        <v>5</v>
+      </c>
+      <c r="U15">
+        <v>5</v>
+      </c>
+      <c r="V15">
+        <v>5</v>
+      </c>
+      <c r="W15" t="s">
+        <v>37</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>20</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" spans="1:26">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16">
+        <v>600</v>
+      </c>
+      <c r="G16">
+        <v>600</v>
+      </c>
+      <c r="H16">
+        <v>600</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>150</v>
+      </c>
+      <c r="L16">
+        <v>80</v>
+      </c>
+      <c r="M16">
+        <v>55000</v>
+      </c>
+      <c r="N16">
+        <v>10000</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>10</v>
+      </c>
+      <c r="Q16">
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <v>10</v>
+      </c>
+      <c r="S16">
+        <v>5</v>
+      </c>
+      <c r="T16">
+        <v>5</v>
+      </c>
+      <c r="U16">
+        <v>5</v>
+      </c>
+      <c r="V16">
+        <v>5</v>
+      </c>
+      <c r="W16" t="s">
+        <v>39</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>20</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" spans="1:26">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17">
+        <v>600</v>
+      </c>
+      <c r="G17">
+        <v>600</v>
+      </c>
+      <c r="H17">
+        <v>600</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>150</v>
+      </c>
+      <c r="L17">
+        <v>80</v>
+      </c>
+      <c r="M17">
+        <v>55000</v>
+      </c>
+      <c r="N17">
+        <v>10000</v>
+      </c>
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <v>10</v>
+      </c>
+      <c r="Q17">
+        <v>10</v>
+      </c>
+      <c r="R17">
+        <v>10</v>
+      </c>
+      <c r="S17">
+        <v>5</v>
+      </c>
+      <c r="T17">
+        <v>5</v>
+      </c>
+      <c r="U17">
+        <v>5</v>
+      </c>
+      <c r="V17">
+        <v>5</v>
+      </c>
+      <c r="W17" t="s">
+        <v>41</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>20</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18">
+        <v>200</v>
+      </c>
+      <c r="G18">
+        <v>200</v>
+      </c>
+      <c r="H18">
+        <v>200</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>50</v>
+      </c>
+      <c r="L18">
+        <v>40</v>
+      </c>
+      <c r="M18">
+        <v>55000</v>
+      </c>
+      <c r="N18">
+        <v>10000</v>
+      </c>
+      <c r="O18">
+        <v>10</v>
+      </c>
+      <c r="P18">
+        <v>10</v>
+      </c>
+      <c r="Q18">
+        <v>10</v>
+      </c>
+      <c r="R18">
+        <v>10</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
+      <c r="T18">
+        <v>5</v>
+      </c>
+      <c r="U18">
+        <v>5</v>
+      </c>
+      <c r="V18">
+        <v>5</v>
+      </c>
+      <c r="W18" t="s">
+        <v>30</v>
+      </c>
+      <c r="X18">
+        <v>2</v>
+      </c>
+      <c r="Y18">
+        <v>20</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19">
+        <v>400</v>
+      </c>
+      <c r="G19">
+        <v>400</v>
+      </c>
+      <c r="H19">
+        <v>400</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>100</v>
+      </c>
+      <c r="L19">
+        <v>60</v>
+      </c>
+      <c r="M19">
+        <v>55000</v>
+      </c>
+      <c r="N19">
+        <v>10000</v>
+      </c>
+      <c r="O19">
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <v>10</v>
+      </c>
+      <c r="Q19">
+        <v>10</v>
+      </c>
+      <c r="R19">
+        <v>10</v>
+      </c>
+      <c r="S19">
+        <v>5</v>
+      </c>
+      <c r="T19">
+        <v>5</v>
+      </c>
+      <c r="U19">
+        <v>5</v>
+      </c>
+      <c r="V19">
+        <v>5</v>
+      </c>
+      <c r="W19" t="s">
+        <v>30</v>
+      </c>
+      <c r="X19">
+        <v>2</v>
+      </c>
+      <c r="Y19">
+        <v>20</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20">
+        <v>600</v>
+      </c>
+      <c r="G20">
+        <v>600</v>
+      </c>
+      <c r="H20">
+        <v>600</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>150</v>
+      </c>
+      <c r="L20">
+        <v>80</v>
+      </c>
+      <c r="M20">
+        <v>55000</v>
+      </c>
+      <c r="N20">
+        <v>10000</v>
+      </c>
+      <c r="O20">
+        <v>10</v>
+      </c>
+      <c r="P20">
+        <v>10</v>
+      </c>
+      <c r="Q20">
+        <v>10</v>
+      </c>
+      <c r="R20">
+        <v>10</v>
+      </c>
+      <c r="S20">
+        <v>5</v>
+      </c>
+      <c r="T20">
+        <v>5</v>
+      </c>
+      <c r="U20">
+        <v>5</v>
+      </c>
+      <c r="V20">
+        <v>5</v>
+      </c>
+      <c r="W20" t="s">
+        <v>30</v>
+      </c>
+      <c r="X20">
+        <v>2</v>
+      </c>
+      <c r="Y20">
+        <v>20</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21">
+        <v>600</v>
+      </c>
+      <c r="G21">
+        <v>600</v>
+      </c>
+      <c r="H21">
+        <v>600</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>150</v>
+      </c>
+      <c r="L21">
+        <v>80</v>
+      </c>
+      <c r="M21">
+        <v>55000</v>
+      </c>
+      <c r="N21">
+        <v>10000</v>
+      </c>
+      <c r="O21">
+        <v>10</v>
+      </c>
+      <c r="P21">
+        <v>10</v>
+      </c>
+      <c r="Q21">
+        <v>10</v>
+      </c>
+      <c r="R21">
+        <v>10</v>
+      </c>
+      <c r="S21">
+        <v>5</v>
+      </c>
+      <c r="T21">
+        <v>5</v>
+      </c>
+      <c r="U21">
+        <v>5</v>
+      </c>
+      <c r="V21">
+        <v>5</v>
+      </c>
+      <c r="W21" t="s">
+        <v>30</v>
+      </c>
+      <c r="X21">
+        <v>2</v>
+      </c>
+      <c r="Y21">
+        <v>20</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
add property for npc
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>ID</t>
   </si>
@@ -146,6 +146,9 @@
     <t>SkillIDRef</t>
   </si>
   <si>
+    <t>Height</t>
+  </si>
+  <si>
     <t>Default</t>
   </si>
   <si>
@@ -245,8 +248,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="2">
@@ -650,10 +653,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -679,9 +682,10 @@
     <col min="24" max="25" width="25" customWidth="1"/>
     <col min="26" max="26" width="13.875" customWidth="1"/>
     <col min="27" max="27" width="14.75" customWidth="1"/>
+    <col min="28" max="28" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,22 +767,25 @@
       <c r="AA1" t="s">
         <v>26</v>
       </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:28">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2">
         <v>600</v>
@@ -832,7 +839,7 @@
         <v>5</v>
       </c>
       <c r="W2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="X2">
         <v>2</v>
@@ -841,24 +848,27 @@
         <v>20</v>
       </c>
       <c r="Z2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="1" spans="1:26">
+    <row r="3" customFormat="1" spans="1:28">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>600</v>
@@ -912,7 +922,7 @@
         <v>5</v>
       </c>
       <c r="W3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -921,24 +931,27 @@
         <v>20</v>
       </c>
       <c r="Z3" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="1" spans="1:26">
+    <row r="4" customFormat="1" spans="1:28">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4">
         <v>600</v>
@@ -992,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="W4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -1001,24 +1014,27 @@
         <v>20</v>
       </c>
       <c r="Z4" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB4">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:26">
+    <row r="5" customFormat="1" spans="1:28">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5">
         <v>600</v>
@@ -1072,7 +1088,7 @@
         <v>5</v>
       </c>
       <c r="W5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X5">
         <v>0</v>
@@ -1081,24 +1097,27 @@
         <v>20</v>
       </c>
       <c r="Z5" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="1" spans="1:26">
+    <row r="6" customFormat="1" spans="1:28">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6">
         <v>600</v>
@@ -1152,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="W6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1161,24 +1180,27 @@
         <v>20</v>
       </c>
       <c r="Z6" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="1" spans="1:26">
+    <row r="7" customFormat="1" spans="1:28">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7">
         <v>600</v>
@@ -1232,7 +1254,7 @@
         <v>5</v>
       </c>
       <c r="W7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -1241,24 +1263,27 @@
         <v>20</v>
       </c>
       <c r="Z7" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB7">
+        <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="1" spans="1:26">
+    <row r="8" customFormat="1" spans="1:28">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <v>600</v>
@@ -1312,7 +1337,7 @@
         <v>5</v>
       </c>
       <c r="W8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -1321,24 +1346,27 @@
         <v>20</v>
       </c>
       <c r="Z8" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB8">
+        <v>2</v>
       </c>
     </row>
-    <row r="9" customFormat="1" spans="1:26">
+    <row r="9" customFormat="1" spans="1:28">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9">
         <v>600</v>
@@ -1392,7 +1420,7 @@
         <v>5</v>
       </c>
       <c r="W9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -1401,24 +1429,27 @@
         <v>20</v>
       </c>
       <c r="Z9" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB9">
+        <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:26">
+    <row r="10" customFormat="1" spans="1:28">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F10">
         <v>600</v>
@@ -1472,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="W10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -1481,24 +1512,27 @@
         <v>20</v>
       </c>
       <c r="Z10" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB10">
+        <v>2</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:26">
+    <row r="11" customFormat="1" spans="1:28">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>600</v>
@@ -1552,7 +1586,7 @@
         <v>5</v>
       </c>
       <c r="W11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -1561,24 +1595,27 @@
         <v>20</v>
       </c>
       <c r="Z11" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:26">
+    <row r="12" customFormat="1" spans="1:28">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12">
         <v>600</v>
@@ -1632,7 +1669,7 @@
         <v>5</v>
       </c>
       <c r="W12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -1641,24 +1678,27 @@
         <v>20</v>
       </c>
       <c r="Z12" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB12">
+        <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:26">
+    <row r="13" customFormat="1" spans="1:28">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13">
         <v>600</v>
@@ -1712,7 +1752,7 @@
         <v>5</v>
       </c>
       <c r="W13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -1721,24 +1761,27 @@
         <v>20</v>
       </c>
       <c r="Z13" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB13">
+        <v>2</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:26">
+    <row r="14" customFormat="1" spans="1:28">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F14">
         <v>600</v>
@@ -1792,7 +1835,7 @@
         <v>5</v>
       </c>
       <c r="W14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X14">
         <v>0</v>
@@ -1801,24 +1844,27 @@
         <v>20</v>
       </c>
       <c r="Z14" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB14">
+        <v>2</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="1:26">
+    <row r="15" customFormat="1" spans="1:28">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F15">
         <v>600</v>
@@ -1872,7 +1918,7 @@
         <v>5</v>
       </c>
       <c r="W15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X15">
         <v>0</v>
@@ -1881,24 +1927,27 @@
         <v>20</v>
       </c>
       <c r="Z15" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB15">
+        <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="1" spans="1:26">
+    <row r="16" customFormat="1" spans="1:28">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F16">
         <v>600</v>
@@ -1952,7 +2001,7 @@
         <v>5</v>
       </c>
       <c r="W16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -1961,24 +2010,27 @@
         <v>20</v>
       </c>
       <c r="Z16" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB16">
+        <v>2</v>
       </c>
     </row>
-    <row r="17" customFormat="1" spans="1:26">
+    <row r="17" customFormat="1" spans="1:28">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F17">
         <v>600</v>
@@ -2032,7 +2084,7 @@
         <v>5</v>
       </c>
       <c r="W17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X17">
         <v>0</v>
@@ -2041,24 +2093,27 @@
         <v>20</v>
       </c>
       <c r="Z17" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB17">
+        <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:28">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F18">
         <v>200</v>
@@ -2112,7 +2167,7 @@
         <v>5</v>
       </c>
       <c r="W18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="X18">
         <v>2</v>
@@ -2121,24 +2176,27 @@
         <v>20</v>
       </c>
       <c r="Z18" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB18">
+        <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:28">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F19">
         <v>400</v>
@@ -2192,7 +2250,7 @@
         <v>5</v>
       </c>
       <c r="W19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="X19">
         <v>2</v>
@@ -2201,24 +2259,27 @@
         <v>20</v>
       </c>
       <c r="Z19" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB19">
+        <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:28">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F20">
         <v>600</v>
@@ -2272,7 +2333,7 @@
         <v>5</v>
       </c>
       <c r="W20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="X20">
         <v>2</v>
@@ -2281,24 +2342,27 @@
         <v>20</v>
       </c>
       <c r="Z20" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB20">
+        <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:28">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F21">
         <v>600</v>
@@ -2352,7 +2416,7 @@
         <v>5</v>
       </c>
       <c r="W21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="X21">
         <v>2</v>
@@ -2361,7 +2425,10 @@
         <v>20</v>
       </c>
       <c r="Z21" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add protocol for mining stone ad npc configuration
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/NPC.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206">
   <si>
     <t>ID</t>
   </si>
@@ -529,6 +529,162 @@
   <si>
     <t>PlayerAtt52</t>
   </si>
+  <si>
+    <t>skeleton_archer_blue</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_archer_blue</t>
+  </si>
+  <si>
+    <t>skeleton_archer_green</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_archer_green</t>
+  </si>
+  <si>
+    <t>skeleton_archer_purple</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_archer_purple</t>
+  </si>
+  <si>
+    <t>skeleton_archer_red</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_archer_red</t>
+  </si>
+  <si>
+    <t>skeleton_archer_teal</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_archer_teal</t>
+  </si>
+  <si>
+    <t>skeleton_archer_yellow</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_archer_yellow</t>
+  </si>
+  <si>
+    <t>skeleton_tom_angry</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_tom_angry</t>
+  </si>
+  <si>
+    <t>skeleton_tom_happy</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_tom_happy</t>
+  </si>
+  <si>
+    <t>skeleton_king_blue</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_king_blue</t>
+  </si>
+  <si>
+    <t>skeleton_king_green</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_king_green</t>
+  </si>
+  <si>
+    <t>skeleton_king_purple</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_king_purple</t>
+  </si>
+  <si>
+    <t>skeleton_king_red</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_king_red</t>
+  </si>
+  <si>
+    <t>skeleton_king_teal</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_king_teal</t>
+  </si>
+  <si>
+    <t>skeleton_king_yellow</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_king_yellow</t>
+  </si>
+  <si>
+    <t>skeleton_mage_blue</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_mage_blue</t>
+  </si>
+  <si>
+    <t>skeleton_mage_green</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_mage_green</t>
+  </si>
+  <si>
+    <t>skeleton_mage_purple</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_mage_purple</t>
+  </si>
+  <si>
+    <t>skeleton_mage_red</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_mage_red</t>
+  </si>
+  <si>
+    <t>skeleton_mage_teal</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_mage_teal</t>
+  </si>
+  <si>
+    <t>skeleton_mage_yellow</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_mage_yellow</t>
+  </si>
+  <si>
+    <t>skeleton_warrior_blue</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_warrior_blue</t>
+  </si>
+  <si>
+    <t>skeleton_warrior_green</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_warrior_green</t>
+  </si>
+  <si>
+    <t>skeleton_warrior_purple</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_warrior_purple</t>
+  </si>
+  <si>
+    <t>skeleton_warrior_red</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_warrior_red</t>
+  </si>
+  <si>
+    <t>skeleton_warrior_teal</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_warrior_teal</t>
+  </si>
+  <si>
+    <t>skeleton_warrior_yellow</t>
+  </si>
+  <si>
+    <t>Prefabs/Object/NPC/skeleton_warrior_yellow</t>
+  </si>
 </sst>
 </file>
 
@@ -540,7 +696,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -549,14 +705,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,9 +747,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -600,8 +786,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,89 +854,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -720,7 +870,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +882,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,19 +948,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -768,97 +1020,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -876,31 +1038,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -914,26 +1064,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -964,9 +1099,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -986,17 +1132,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1011,153 +1146,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1559,10 +1709,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:F53"/>
+    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53:J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3118,6 +3268,685 @@
         <v>14</v>
       </c>
     </row>
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54">
+        <v>52</v>
+      </c>
+      <c r="C54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>20</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>20</v>
+      </c>
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>20</v>
+      </c>
+      <c r="F57" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>20</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>20</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>20</v>
+      </c>
+      <c r="F60" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>20</v>
+      </c>
+      <c r="F61" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61">
+        <v>2</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" t="s">
+        <v>171</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>20</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62">
+        <v>2</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" t="s">
+        <v>173</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>20</v>
+      </c>
+      <c r="F63" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" t="s">
+        <v>174</v>
+      </c>
+      <c r="C64" t="s">
+        <v>175</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>20</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64">
+        <v>2</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" t="s">
+        <v>176</v>
+      </c>
+      <c r="C65" t="s">
+        <v>177</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>20</v>
+      </c>
+      <c r="F65" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65">
+        <v>2</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" t="s">
+        <v>179</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>20</v>
+      </c>
+      <c r="F66" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" t="s">
+        <v>180</v>
+      </c>
+      <c r="C67" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>20</v>
+      </c>
+      <c r="F67" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" t="s">
+        <v>182</v>
+      </c>
+      <c r="C68" t="s">
+        <v>183</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>20</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" t="s">
+        <v>184</v>
+      </c>
+      <c r="C69" t="s">
+        <v>185</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>20</v>
+      </c>
+      <c r="F69" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69">
+        <v>2</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" t="s">
+        <v>186</v>
+      </c>
+      <c r="C70" t="s">
+        <v>187</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>20</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70">
+        <v>2</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" t="s">
+        <v>188</v>
+      </c>
+      <c r="C71" t="s">
+        <v>189</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>20</v>
+      </c>
+      <c r="F71" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" t="s">
+        <v>190</v>
+      </c>
+      <c r="C72" t="s">
+        <v>191</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>20</v>
+      </c>
+      <c r="F72" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72">
+        <v>2</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" t="s">
+        <v>192</v>
+      </c>
+      <c r="C73" t="s">
+        <v>193</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>20</v>
+      </c>
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" t="s">
+        <v>194</v>
+      </c>
+      <c r="C74" t="s">
+        <v>195</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>20</v>
+      </c>
+      <c r="F74" t="s">
+        <v>12</v>
+      </c>
+      <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" t="s">
+        <v>196</v>
+      </c>
+      <c r="C75" t="s">
+        <v>197</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>20</v>
+      </c>
+      <c r="F75" t="s">
+        <v>12</v>
+      </c>
+      <c r="H75">
+        <v>2</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J75" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" t="s">
+        <v>198</v>
+      </c>
+      <c r="C76" t="s">
+        <v>199</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>20</v>
+      </c>
+      <c r="F76" t="s">
+        <v>12</v>
+      </c>
+      <c r="H76">
+        <v>2</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" t="s">
+        <v>200</v>
+      </c>
+      <c r="C77" t="s">
+        <v>201</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <v>20</v>
+      </c>
+      <c r="F77" t="s">
+        <v>12</v>
+      </c>
+      <c r="H77">
+        <v>2</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J77" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" t="s">
+        <v>202</v>
+      </c>
+      <c r="C78" t="s">
+        <v>203</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>20</v>
+      </c>
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" t="s">
+        <v>204</v>
+      </c>
+      <c r="C79" t="s">
+        <v>205</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>20</v>
+      </c>
+      <c r="F79" t="s">
+        <v>12</v>
+      </c>
+      <c r="H79">
+        <v>2</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J79" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>